<commit_message>
Update multiverse analysis figures and scripts
</commit_message>
<xml_diff>
--- a/qol_specs_results_summary_df.xlsx
+++ b/qol_specs_results_summary_df.xlsx
@@ -614,22 +614,22 @@
         </is>
       </c>
       <c r="C8">
-        <v>0.08081125953220593</v>
+        <v>0.14814730973738</v>
       </c>
       <c r="D8">
-        <v>0.03145285437101755</v>
+        <v>0.01810307127738879</v>
       </c>
       <c r="E8">
-        <v>0.04580630827642475</v>
+        <v>0.1240665813995394</v>
       </c>
       <c r="F8">
-        <v>0.1194602848723428</v>
+        <v>0.1736406001703299</v>
       </c>
       <c r="G8">
-        <v>0.06107828339163594</v>
+        <v>0.134271690424067</v>
       </c>
       <c r="H8">
-        <v>0.10045436436044</v>
+        <v>0.1596206999675694</v>
       </c>
       <c r="I8">
         <v>159</v>
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="C9">
-        <v>0.198671892656628</v>
+        <v>0.2606213405587098</v>
       </c>
       <c r="D9">
-        <v>0.01446151295917701</v>
+        <v>0.01001885071711333</v>
       </c>
       <c r="E9">
-        <v>0.1649792149343142</v>
+        <v>0.232093937381568</v>
       </c>
       <c r="F9">
-        <v>0.2194186353142481</v>
+        <v>0.2747122803586632</v>
       </c>
       <c r="G9">
-        <v>0.1892342111755293</v>
+        <v>0.2515655372898408</v>
       </c>
       <c r="H9">
-        <v>0.2089059193560689</v>
+        <v>0.2665331144783281</v>
       </c>
       <c r="I9">
         <v>159</v>
@@ -680,22 +680,22 @@
         </is>
       </c>
       <c r="C10">
-        <v>0.1771530476218103</v>
+        <v>0.242901726420291</v>
       </c>
       <c r="D10">
-        <v>0.02200723600781501</v>
+        <v>0.01520806452611467</v>
       </c>
       <c r="E10">
-        <v>0.1277367675525222</v>
+        <v>0.2022570932042213</v>
       </c>
       <c r="F10">
-        <v>0.2200497622288238</v>
+        <v>0.2725805542232504</v>
       </c>
       <c r="G10">
-        <v>0.1647507391496107</v>
+        <v>0.2339862158571543</v>
       </c>
       <c r="H10">
-        <v>0.1922355660037879</v>
+        <v>0.2535812536075055</v>
       </c>
       <c r="I10">
         <v>159</v>

</xml_diff>